<commit_message>
Describing your data activity and planning out visualizations
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58534D85-ED85-544E-BD4B-5F5089D19D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE4E416-77E2-644F-AD5E-3A7BE1FE2135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="3820" windowWidth="28040" windowHeight="15820" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Identified questions to answer with the data</t>
+  </si>
+  <si>
+    <t>Describing your data</t>
   </si>
 </sst>
 </file>
@@ -84,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,6 +446,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44592</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial data visualization and R tinkering
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E8FB07-C809-FD49-B96C-D42DF946F060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF34DA50-C0C2-CD43-8773-5FD47A0B41E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Initial framework for a scatterplot between consumption and renewable energy production</t>
+  </si>
+  <si>
+    <t>Built a scatterplot and a Shiny app!</t>
   </si>
 </sst>
 </file>
@@ -90,10 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,19 +414,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -431,7 +440,7 @@
       <c r="A2" s="1">
         <v>44590</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>0.5</v>
       </c>
       <c r="C2" t="s">
@@ -442,7 +451,7 @@
       <c r="A3" s="1">
         <v>44591</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.5</v>
       </c>
       <c r="C3" t="s">
@@ -453,7 +462,7 @@
       <c r="A4" s="2">
         <v>44592</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" t="s">
@@ -464,11 +473,22 @@
       <c r="A5" s="2">
         <v>44592</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44593</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further experimentation. Got it set up so you click on the scatterplot and the country name appears below
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF34DA50-C0C2-CD43-8773-5FD47A0B41E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25473644-46E7-E648-9FE7-29DA0688DC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Built a scatterplot and a Shiny app!</t>
+  </si>
+  <si>
+    <t>Experimenting with displays, hover to display, click to display</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,6 +494,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>44600</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Feb 13: Adding line chart, data manipulation
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25473644-46E7-E648-9FE7-29DA0688DC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAA24A4-01C2-7748-BAA3-20BC8A2EE97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Experimenting with displays, hover to display, click to display</t>
+  </si>
+  <si>
+    <t>Adding a line chart to help understand trends over time</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,6 +508,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>44605</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Layout + color tweaks
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAA24A4-01C2-7748-BAA3-20BC8A2EE97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4FED56-5F83-344A-AE1A-59A7E77DBA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Adding a line chart to help understand trends over time</t>
+  </si>
+  <si>
+    <t>Display stuff, fixing issues with pie chart</t>
+  </si>
+  <si>
+    <t>Colors, title, alignment</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,6 +525,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>44606</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>44607</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating documentation and positioning of plots
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC19BC2-07DF-0D43-BE74-17352F5C6A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB212B-0C18-B342-A992-5CB95F424144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Worked on alignment etc, added area chart</t>
+  </si>
+  <si>
+    <t>Updating positioning and documentation</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,6 +564,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>44614</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
additional scatter plot, highlighting outliers
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F82E00-C5CD-334B-8CF9-22FE62E5E8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C805B2-17F7-3148-BE2D-3C2F8A3432BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Documentation, planning</t>
+  </si>
+  <si>
+    <t>Adding another scatter plot, highlighting outliers</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,6 +592,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>44616</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more documentation and formatting
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298D88F4-C00A-4043-9D4A-7563DA0A0C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938E56C9-83F1-CF4E-8C30-CC74A1109C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>descriptions</t>
+  </si>
+  <si>
+    <t>formatting, descriptions</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,6 +634,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>44622</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Proper documentation and code clean up
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahfehr/Documents/CSC-324/324-individual-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3782E10E-C75D-B848-8302-ABA8473526C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE2E85A-3B66-3C4B-9E4E-7B641EC8B33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15780" xr2:uid="{C7949DF2-3895-5D48-B602-842BE04AEE8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Word cloud</t>
+  </si>
+  <si>
+    <t>Proper Documentation</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330168A-0701-524F-83AF-9976297AE332}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,6 +704,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>44632</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>